<commit_message>
Sun Dec 22 08:21:02 PM EST 2024
</commit_message>
<xml_diff>
--- a/ozone/MAE_stacked.xlsx
+++ b/ozone/MAE_stacked.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09798757153841207</v>
+        <v>0.3771839289624588</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7301515166201069</v>
+        <v>3.334164874200428</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1047583938750073</v>
+        <v>0.3929637689979964</v>
       </c>
       <c r="C3" t="n">
-        <v>1.102359249518327</v>
+        <v>4.399788092463178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mon Dec 23 09:41:49 PM EST 2024
</commit_message>
<xml_diff>
--- a/ozone/MAE_stacked.xlsx
+++ b/ozone/MAE_stacked.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3771839289624588</v>
+        <v>0.2851076882107093</v>
       </c>
       <c r="C2" t="n">
-        <v>3.334164874200428</v>
+        <v>2.671180954222684</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3929637689979964</v>
+        <v>0.2991427698894775</v>
       </c>
       <c r="C3" t="n">
-        <v>4.399788092463178</v>
+        <v>3.086674271150811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>